<commit_message>
Added sensitivities and profiles, exec. summary
</commit_message>
<xml_diff>
--- a/txt_files/Fleet9_CCFRP_IndexData.xlsx
+++ b/txt_files/Fleet9_CCFRP_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16037" windowHeight="6514" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16037" windowHeight="6514"/>
   </bookViews>
   <sheets>
     <sheet name="AIC" sheetId="1" r:id="rId1"/>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -481,12 +481,6 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -497,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>